<commit_message>
More troubleshooting tweaks. Including: - Implemented real warning messages and improved their clarity - Most error handling is now done by validateMatrix()
</commit_message>
<xml_diff>
--- a/inst/extdata/DibamidaeDemo.xlsx
+++ b/inst/extdata/DibamidaeDemo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User1\Syncthing-Docs\Dissertation\Scalation Networks\pholidosis\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D738AF2-8D62-4C40-B77E-0038C4D1DE1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18745F1F-A9CC-4C99-95EA-4DE2FCEB1A4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Anelytropsis_papillosus" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -215,7 +215,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -232,6 +232,18 @@
       <patternFill patternType="solid">
         <fgColor theme="2"/>
         <bgColor theme="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -364,7 +376,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -392,6 +404,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1919,10 +1936,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AM39"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AA1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="H15" sqref="H15"/>
-      <selection pane="topRight" activeCell="AI40" sqref="AI40"/>
+      <selection pane="topRight" activeCell="AM39" sqref="A1:AM39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1951,364 +1968,369 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="A1" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="D1" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="F1" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="V1" t="s">
+      <c r="V1" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="W1" t="s">
+      <c r="W1" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="X1" t="s">
+      <c r="X1" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Y1" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="Z1" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AA1" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AB1" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AC1" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AD1" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AE1" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AF1" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AG1" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AH1" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AI1" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AJ1" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AK1" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AL1" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AM1" s="27" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="D2" cm="1">
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27" cm="1">
         <f t="array" ref="D2:AM3">TRANSPOSE(B4:C39)</f>
         <v>1</v>
       </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-      <c r="O2">
-        <v>1</v>
-      </c>
-      <c r="P2">
-        <v>1</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-      <c r="T2">
-        <v>1</v>
-      </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-      <c r="V2">
-        <v>0</v>
-      </c>
-      <c r="W2">
-        <v>0</v>
-      </c>
-      <c r="X2">
-        <v>0</v>
-      </c>
-      <c r="Y2">
-        <v>0</v>
-      </c>
-      <c r="Z2">
-        <v>0</v>
-      </c>
-      <c r="AA2">
-        <v>0</v>
-      </c>
-      <c r="AB2">
-        <v>1</v>
-      </c>
-      <c r="AC2">
-        <v>1</v>
-      </c>
-      <c r="AD2">
-        <v>1</v>
-      </c>
-      <c r="AE2">
-        <v>1</v>
-      </c>
-      <c r="AF2">
-        <v>0</v>
-      </c>
-      <c r="AG2">
-        <v>0</v>
-      </c>
-      <c r="AH2">
-        <v>0</v>
-      </c>
-      <c r="AI2">
-        <v>1</v>
-      </c>
-      <c r="AJ2">
-        <v>0</v>
-      </c>
-      <c r="AK2">
-        <v>0</v>
-      </c>
-      <c r="AL2">
-        <v>0</v>
-      </c>
-      <c r="AM2">
+      <c r="E2" s="27">
+        <v>0</v>
+      </c>
+      <c r="F2" s="27">
+        <v>0</v>
+      </c>
+      <c r="G2" s="27">
+        <v>0</v>
+      </c>
+      <c r="H2" s="27">
+        <v>1</v>
+      </c>
+      <c r="I2" s="27">
+        <v>0</v>
+      </c>
+      <c r="J2" s="27">
+        <v>0</v>
+      </c>
+      <c r="K2" s="27">
+        <v>0</v>
+      </c>
+      <c r="L2" s="27">
+        <v>0</v>
+      </c>
+      <c r="M2" s="27">
+        <v>1</v>
+      </c>
+      <c r="N2" s="27">
+        <v>1</v>
+      </c>
+      <c r="O2" s="27">
+        <v>1</v>
+      </c>
+      <c r="P2" s="27">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="27">
+        <v>0</v>
+      </c>
+      <c r="R2" s="27">
+        <v>0</v>
+      </c>
+      <c r="S2" s="27">
+        <v>0</v>
+      </c>
+      <c r="T2" s="27">
+        <v>1</v>
+      </c>
+      <c r="U2" s="27">
+        <v>0</v>
+      </c>
+      <c r="V2" s="27">
+        <v>0</v>
+      </c>
+      <c r="W2" s="27">
+        <v>0</v>
+      </c>
+      <c r="X2" s="27">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="27">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="27">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="27">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="27">
+        <v>1</v>
+      </c>
+      <c r="AC2" s="27">
+        <v>1</v>
+      </c>
+      <c r="AD2" s="27">
+        <v>1</v>
+      </c>
+      <c r="AE2" s="27">
+        <v>1</v>
+      </c>
+      <c r="AF2" s="27">
+        <v>0</v>
+      </c>
+      <c r="AG2" s="27">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="27">
+        <v>0</v>
+      </c>
+      <c r="AI2" s="27">
+        <v>1</v>
+      </c>
+      <c r="AJ2" s="27">
+        <v>0</v>
+      </c>
+      <c r="AK2" s="27">
+        <v>0</v>
+      </c>
+      <c r="AL2" s="27">
+        <v>0</v>
+      </c>
+      <c r="AM2" s="27">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3">
-        <v>1</v>
-      </c>
-      <c r="Q3">
-        <v>1</v>
-      </c>
-      <c r="R3">
-        <v>1</v>
-      </c>
-      <c r="S3">
-        <v>1</v>
-      </c>
-      <c r="T3">
-        <v>0</v>
-      </c>
-      <c r="U3">
-        <v>1</v>
-      </c>
-      <c r="V3">
-        <v>1</v>
-      </c>
-      <c r="W3">
-        <v>1</v>
-      </c>
-      <c r="X3">
-        <v>1</v>
-      </c>
-      <c r="Y3">
-        <v>0</v>
-      </c>
-      <c r="Z3">
-        <v>0</v>
-      </c>
-      <c r="AA3">
-        <v>0</v>
-      </c>
-      <c r="AB3">
-        <v>0</v>
-      </c>
-      <c r="AC3">
-        <v>0</v>
-      </c>
-      <c r="AD3">
-        <v>0</v>
-      </c>
-      <c r="AE3">
-        <v>1</v>
-      </c>
-      <c r="AF3">
-        <v>1</v>
-      </c>
-      <c r="AG3">
-        <v>1</v>
-      </c>
-      <c r="AH3">
-        <v>1</v>
-      </c>
-      <c r="AI3">
-        <v>0</v>
-      </c>
-      <c r="AJ3">
-        <v>1</v>
-      </c>
-      <c r="AK3">
-        <v>1</v>
-      </c>
-      <c r="AL3">
-        <v>1</v>
-      </c>
-      <c r="AM3">
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27">
+        <v>0</v>
+      </c>
+      <c r="E3" s="27">
+        <v>0</v>
+      </c>
+      <c r="F3" s="27">
+        <v>0</v>
+      </c>
+      <c r="G3" s="27">
+        <v>1</v>
+      </c>
+      <c r="H3" s="27">
+        <v>0</v>
+      </c>
+      <c r="I3" s="27">
+        <v>1</v>
+      </c>
+      <c r="J3" s="27">
+        <v>0</v>
+      </c>
+      <c r="K3" s="27">
+        <v>0</v>
+      </c>
+      <c r="L3" s="27">
+        <v>0</v>
+      </c>
+      <c r="M3" s="27">
+        <v>0</v>
+      </c>
+      <c r="N3" s="27">
+        <v>0</v>
+      </c>
+      <c r="O3" s="27">
+        <v>0</v>
+      </c>
+      <c r="P3" s="27">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="27">
+        <v>1</v>
+      </c>
+      <c r="R3" s="27">
+        <v>1</v>
+      </c>
+      <c r="S3" s="27">
+        <v>1</v>
+      </c>
+      <c r="T3" s="27">
+        <v>0</v>
+      </c>
+      <c r="U3" s="27">
+        <v>1</v>
+      </c>
+      <c r="V3" s="27">
+        <v>1</v>
+      </c>
+      <c r="W3" s="27">
+        <v>1</v>
+      </c>
+      <c r="X3" s="27">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="27">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="27">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="27">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="27">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="27">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="27">
+        <v>1</v>
+      </c>
+      <c r="AF3" s="27">
+        <v>1</v>
+      </c>
+      <c r="AG3" s="27">
+        <v>1</v>
+      </c>
+      <c r="AH3" s="27">
+        <v>1</v>
+      </c>
+      <c r="AI3" s="27">
+        <v>0</v>
+      </c>
+      <c r="AJ3" s="27">
+        <v>1</v>
+      </c>
+      <c r="AK3" s="27">
+        <v>1</v>
+      </c>
+      <c r="AL3" s="27">
+        <v>1</v>
+      </c>
+      <c r="AM3" s="27">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
+      <c r="A4" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="27">
+        <v>1</v>
+      </c>
+      <c r="C4" s="27"/>
       <c r="D4" s="4"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
+      <c r="I4" s="6"/>
       <c r="J4" s="7">
         <v>3</v>
       </c>
@@ -2327,8 +2349,8 @@
       <c r="U4" s="5"/>
       <c r="V4" s="5"/>
       <c r="W4" s="5"/>
-      <c r="X4" s="5"/>
-      <c r="Y4" s="7">
+      <c r="X4" s="6"/>
+      <c r="Y4" s="5">
         <v>3</v>
       </c>
       <c r="Z4" s="5"/>
@@ -2345,120 +2367,233 @@
       <c r="AI4" s="5"/>
       <c r="AJ4" s="5"/>
       <c r="AK4" s="5"/>
-      <c r="AL4" s="6"/>
+      <c r="AL4" s="5"/>
+      <c r="AM4" s="6"/>
     </row>
     <row r="5" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="27" t="s">
         <v>2</v>
       </c>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
       <c r="D5" s="8"/>
-      <c r="E5" s="1"/>
-      <c r="F5">
-        <v>1</v>
-      </c>
+      <c r="E5" s="28"/>
+      <c r="F5" s="27">
+        <v>1</v>
+      </c>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="3"/>
       <c r="J5" s="8">
         <v>1</v>
       </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-      <c r="Y5" s="8">
-        <v>1</v>
-      </c>
-      <c r="Z5">
-        <v>1</v>
-      </c>
-      <c r="AA5">
-        <v>1</v>
-      </c>
-      <c r="AL5" s="3"/>
+      <c r="K5" s="27">
+        <v>1</v>
+      </c>
+      <c r="L5" s="27">
+        <v>1</v>
+      </c>
+      <c r="M5" s="27"/>
+      <c r="N5" s="27"/>
+      <c r="O5" s="27"/>
+      <c r="P5" s="27"/>
+      <c r="Q5" s="27"/>
+      <c r="R5" s="27"/>
+      <c r="S5" s="27"/>
+      <c r="T5" s="27"/>
+      <c r="U5" s="27"/>
+      <c r="V5" s="27"/>
+      <c r="W5" s="27"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="27">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="27">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="27">
+        <v>1</v>
+      </c>
+      <c r="AB5" s="27"/>
+      <c r="AC5" s="27"/>
+      <c r="AD5" s="27"/>
+      <c r="AE5" s="27"/>
+      <c r="AF5" s="27"/>
+      <c r="AG5" s="27"/>
+      <c r="AH5" s="27"/>
+      <c r="AI5" s="27"/>
+      <c r="AJ5" s="27"/>
+      <c r="AK5" s="27"/>
+      <c r="AL5" s="27"/>
+      <c r="AM5" s="3"/>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
+      <c r="A6" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
       <c r="D6" s="8"/>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6" s="1"/>
-      <c r="G6">
-        <v>1</v>
-      </c>
+      <c r="E6" s="27">
+        <v>1</v>
+      </c>
+      <c r="F6" s="28"/>
+      <c r="G6" s="27">
+        <v>1</v>
+      </c>
+      <c r="H6" s="27"/>
+      <c r="I6" s="3"/>
       <c r="J6" s="8"/>
-      <c r="L6">
-        <v>1</v>
-      </c>
-      <c r="Q6">
-        <v>1</v>
-      </c>
-      <c r="S6">
-        <v>1</v>
-      </c>
-      <c r="Y6" s="8"/>
-      <c r="AA6">
-        <v>1</v>
-      </c>
-      <c r="AF6">
-        <v>1</v>
-      </c>
-      <c r="AH6">
-        <v>1</v>
-      </c>
-      <c r="AL6" s="3"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="27">
+        <v>1</v>
+      </c>
+      <c r="M6" s="27"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="27"/>
+      <c r="P6" s="27"/>
+      <c r="Q6" s="27">
+        <v>1</v>
+      </c>
+      <c r="R6" s="27"/>
+      <c r="S6" s="27">
+        <v>1</v>
+      </c>
+      <c r="T6" s="27"/>
+      <c r="U6" s="27"/>
+      <c r="V6" s="27"/>
+      <c r="W6" s="27"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="27"/>
+      <c r="Z6" s="27"/>
+      <c r="AA6" s="27">
+        <v>1</v>
+      </c>
+      <c r="AB6" s="27"/>
+      <c r="AC6" s="27"/>
+      <c r="AD6" s="27"/>
+      <c r="AE6" s="27"/>
+      <c r="AF6" s="27">
+        <v>1</v>
+      </c>
+      <c r="AG6" s="27"/>
+      <c r="AH6" s="27">
+        <v>1</v>
+      </c>
+      <c r="AI6" s="27"/>
+      <c r="AJ6" s="27"/>
+      <c r="AK6" s="27"/>
+      <c r="AL6" s="27"/>
+      <c r="AM6" s="3"/>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C7">
+      <c r="B7" s="27"/>
+      <c r="C7" s="27">
         <v>1</v>
       </c>
       <c r="D7" s="8"/>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7" s="1"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27">
+        <v>1</v>
+      </c>
+      <c r="G7" s="28"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="3"/>
       <c r="J7" s="8"/>
-      <c r="S7">
-        <v>1</v>
-      </c>
-      <c r="Y7" s="8"/>
-      <c r="AH7">
-        <v>1</v>
-      </c>
-      <c r="AL7" s="3"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="27"/>
+      <c r="O7" s="27"/>
+      <c r="P7" s="27"/>
+      <c r="Q7" s="27"/>
+      <c r="R7" s="27"/>
+      <c r="S7" s="27">
+        <v>1</v>
+      </c>
+      <c r="T7" s="27"/>
+      <c r="U7" s="27"/>
+      <c r="V7" s="27"/>
+      <c r="W7" s="27"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="27"/>
+      <c r="Z7" s="27"/>
+      <c r="AA7" s="27"/>
+      <c r="AB7" s="27"/>
+      <c r="AC7" s="27"/>
+      <c r="AD7" s="27"/>
+      <c r="AE7" s="27"/>
+      <c r="AF7" s="27"/>
+      <c r="AG7" s="27"/>
+      <c r="AH7" s="27">
+        <v>1</v>
+      </c>
+      <c r="AI7" s="27"/>
+      <c r="AJ7" s="27"/>
+      <c r="AK7" s="27"/>
+      <c r="AL7" s="27"/>
+      <c r="AM7" s="3"/>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
+      <c r="B8" s="27">
+        <v>1</v>
+      </c>
+      <c r="C8" s="27"/>
       <c r="D8" s="8"/>
-      <c r="H8" s="1"/>
-      <c r="I8">
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="3">
         <v>1</v>
       </c>
       <c r="J8" s="8"/>
-      <c r="T8">
-        <v>1</v>
-      </c>
-      <c r="Y8" s="8"/>
-      <c r="AI8">
-        <v>1</v>
-      </c>
-      <c r="AL8" s="3"/>
+      <c r="K8" s="27"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="27"/>
+      <c r="N8" s="27"/>
+      <c r="O8" s="27"/>
+      <c r="P8" s="27"/>
+      <c r="Q8" s="27"/>
+      <c r="R8" s="27"/>
+      <c r="S8" s="27"/>
+      <c r="T8" s="27">
+        <v>1</v>
+      </c>
+      <c r="U8" s="27"/>
+      <c r="V8" s="27"/>
+      <c r="W8" s="27"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="27"/>
+      <c r="Z8" s="27"/>
+      <c r="AA8" s="27"/>
+      <c r="AB8" s="27"/>
+      <c r="AC8" s="27"/>
+      <c r="AD8" s="27"/>
+      <c r="AE8" s="27"/>
+      <c r="AF8" s="27"/>
+      <c r="AG8" s="27"/>
+      <c r="AH8" s="27"/>
+      <c r="AI8" s="27">
+        <v>1</v>
+      </c>
+      <c r="AJ8" s="27"/>
+      <c r="AK8" s="27"/>
+      <c r="AL8" s="27"/>
+      <c r="AM8" s="3"/>
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="C9">
+      <c r="B9" s="27"/>
+      <c r="C9" s="27">
         <v>1</v>
       </c>
       <c r="D9" s="9"/>
@@ -2470,7 +2605,7 @@
       <c r="H9" s="2">
         <v>1</v>
       </c>
-      <c r="I9" s="19"/>
+      <c r="I9" s="10"/>
       <c r="J9" s="9"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
@@ -2489,8 +2624,8 @@
       </c>
       <c r="V9" s="2"/>
       <c r="W9" s="2"/>
-      <c r="X9" s="2"/>
-      <c r="Y9" s="9"/>
+      <c r="X9" s="11"/>
+      <c r="Y9" s="2"/>
       <c r="Z9" s="2"/>
       <c r="AA9" s="2"/>
       <c r="AB9" s="2"/>
@@ -2507,1160 +2642,1602 @@
         <v>1</v>
       </c>
       <c r="AK9" s="2"/>
-      <c r="AL9" s="11"/>
+      <c r="AL9" s="2"/>
+      <c r="AM9" s="11"/>
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="8">
-        <v>3</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="J10" s="17"/>
-      <c r="K10" s="8">
-        <v>3</v>
-      </c>
-      <c r="M10">
-        <v>3</v>
-      </c>
-      <c r="W10" s="3"/>
-      <c r="Y10" s="14">
-        <v>3</v>
-      </c>
-      <c r="Z10" s="15"/>
-      <c r="AA10" s="15"/>
-      <c r="AB10" s="15"/>
-      <c r="AC10" s="15"/>
-      <c r="AD10" s="15"/>
-      <c r="AE10" s="15"/>
-      <c r="AF10" s="15"/>
-      <c r="AG10" s="15"/>
-      <c r="AH10" s="15"/>
-      <c r="AI10" s="15"/>
-      <c r="AJ10" s="15"/>
-      <c r="AK10" s="15"/>
-      <c r="AL10" s="18"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="7">
+        <v>3</v>
+      </c>
+      <c r="E10" s="5">
+        <v>1</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="27">
+        <v>3</v>
+      </c>
+      <c r="L10" s="27"/>
+      <c r="M10" s="27">
+        <v>3</v>
+      </c>
+      <c r="N10" s="27"/>
+      <c r="O10" s="27"/>
+      <c r="P10" s="27"/>
+      <c r="Q10" s="27"/>
+      <c r="R10" s="27"/>
+      <c r="S10" s="27"/>
+      <c r="T10" s="27"/>
+      <c r="U10" s="27"/>
+      <c r="V10" s="27"/>
+      <c r="W10" s="27"/>
+      <c r="X10" s="27"/>
+      <c r="Y10" s="29">
+        <v>3</v>
+      </c>
+      <c r="Z10" s="29"/>
+      <c r="AA10" s="29"/>
+      <c r="AB10" s="29"/>
+      <c r="AC10" s="29"/>
+      <c r="AD10" s="29"/>
+      <c r="AE10" s="29"/>
+      <c r="AF10" s="29"/>
+      <c r="AG10" s="29"/>
+      <c r="AH10" s="29"/>
+      <c r="AI10" s="29"/>
+      <c r="AJ10" s="29"/>
+      <c r="AK10" s="29"/>
+      <c r="AL10" s="29"/>
+      <c r="AM10" s="30"/>
     </row>
     <row r="11" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="27" t="s">
         <v>8</v>
       </c>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
       <c r="D11" s="8"/>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="J11" s="8">
-        <v>3</v>
-      </c>
-      <c r="K11" s="1"/>
-      <c r="L11">
-        <v>1</v>
-      </c>
-      <c r="M11">
-        <v>3</v>
-      </c>
-      <c r="N11">
-        <v>1</v>
-      </c>
-      <c r="W11" s="3"/>
-      <c r="Y11" s="14"/>
-      <c r="Z11" s="15"/>
-      <c r="AA11" s="15"/>
-      <c r="AB11" s="15"/>
-      <c r="AC11" s="15"/>
-      <c r="AD11" s="15"/>
-      <c r="AE11" s="15"/>
-      <c r="AF11" s="15"/>
-      <c r="AG11" s="15"/>
-      <c r="AH11" s="15"/>
-      <c r="AI11" s="15"/>
-      <c r="AJ11" s="15"/>
-      <c r="AK11" s="15"/>
-      <c r="AL11" s="18"/>
+      <c r="E11" s="27">
+        <v>1</v>
+      </c>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="27">
+        <v>3</v>
+      </c>
+      <c r="K11" s="28"/>
+      <c r="L11" s="27">
+        <v>1</v>
+      </c>
+      <c r="M11" s="27">
+        <v>3</v>
+      </c>
+      <c r="N11" s="27">
+        <v>1</v>
+      </c>
+      <c r="O11" s="27"/>
+      <c r="P11" s="27"/>
+      <c r="Q11" s="27"/>
+      <c r="R11" s="27"/>
+      <c r="S11" s="27"/>
+      <c r="T11" s="27"/>
+      <c r="U11" s="27"/>
+      <c r="V11" s="27"/>
+      <c r="W11" s="27"/>
+      <c r="X11" s="27"/>
+      <c r="Y11" s="29"/>
+      <c r="Z11" s="29"/>
+      <c r="AA11" s="29"/>
+      <c r="AB11" s="29"/>
+      <c r="AC11" s="29"/>
+      <c r="AD11" s="29"/>
+      <c r="AE11" s="29"/>
+      <c r="AF11" s="29"/>
+      <c r="AG11" s="29"/>
+      <c r="AH11" s="29"/>
+      <c r="AI11" s="29"/>
+      <c r="AJ11" s="29"/>
+      <c r="AK11" s="29"/>
+      <c r="AL11" s="29"/>
+      <c r="AM11" s="30"/>
     </row>
     <row r="12" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="27" t="s">
         <v>9</v>
       </c>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
       <c r="D12" s="8"/>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="J12" s="8"/>
-      <c r="K12">
-        <v>1</v>
-      </c>
-      <c r="L12" s="1"/>
-      <c r="N12">
-        <v>1</v>
-      </c>
-      <c r="O12">
-        <v>1</v>
-      </c>
-      <c r="P12">
-        <v>1</v>
-      </c>
-      <c r="Q12">
-        <v>1</v>
-      </c>
-      <c r="R12">
-        <v>1</v>
-      </c>
-      <c r="W12" s="3"/>
-      <c r="Y12" s="14"/>
-      <c r="Z12" s="15"/>
-      <c r="AA12" s="15"/>
-      <c r="AB12" s="15"/>
-      <c r="AC12" s="15"/>
-      <c r="AD12" s="15"/>
-      <c r="AE12" s="15"/>
-      <c r="AF12" s="15"/>
-      <c r="AG12" s="15"/>
-      <c r="AH12" s="15"/>
-      <c r="AI12" s="15"/>
-      <c r="AJ12" s="15"/>
-      <c r="AK12" s="15"/>
-      <c r="AL12" s="18"/>
+      <c r="E12" s="27">
+        <v>1</v>
+      </c>
+      <c r="F12" s="27">
+        <v>1</v>
+      </c>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27">
+        <v>1</v>
+      </c>
+      <c r="L12" s="28"/>
+      <c r="M12" s="27"/>
+      <c r="N12" s="27">
+        <v>1</v>
+      </c>
+      <c r="O12" s="27">
+        <v>1</v>
+      </c>
+      <c r="P12" s="27">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="27">
+        <v>1</v>
+      </c>
+      <c r="R12" s="27">
+        <v>1</v>
+      </c>
+      <c r="S12" s="27"/>
+      <c r="T12" s="27"/>
+      <c r="U12" s="27"/>
+      <c r="V12" s="27"/>
+      <c r="W12" s="27"/>
+      <c r="X12" s="27"/>
+      <c r="Y12" s="29"/>
+      <c r="Z12" s="29"/>
+      <c r="AA12" s="29"/>
+      <c r="AB12" s="29"/>
+      <c r="AC12" s="29"/>
+      <c r="AD12" s="29"/>
+      <c r="AE12" s="29"/>
+      <c r="AF12" s="29"/>
+      <c r="AG12" s="29"/>
+      <c r="AH12" s="29"/>
+      <c r="AI12" s="29"/>
+      <c r="AJ12" s="29"/>
+      <c r="AK12" s="29"/>
+      <c r="AL12" s="29"/>
+      <c r="AM12" s="30"/>
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
+      <c r="B13" s="27">
+        <v>1</v>
+      </c>
+      <c r="C13" s="27"/>
       <c r="D13" s="8">
         <v>3</v>
       </c>
-      <c r="J13" s="8">
-        <v>3</v>
-      </c>
-      <c r="K13">
-        <v>3</v>
-      </c>
-      <c r="M13" s="1"/>
-      <c r="N13">
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="27">
+        <v>3</v>
+      </c>
+      <c r="K13" s="27">
+        <v>3</v>
+      </c>
+      <c r="L13" s="27"/>
+      <c r="M13" s="28"/>
+      <c r="N13" s="27">
         <v>2</v>
       </c>
-      <c r="W13" s="3"/>
-      <c r="Y13" s="14"/>
-      <c r="Z13" s="15"/>
-      <c r="AA13" s="15"/>
-      <c r="AB13" s="15"/>
-      <c r="AC13" s="15"/>
-      <c r="AD13" s="15"/>
-      <c r="AE13" s="15"/>
-      <c r="AF13" s="15"/>
-      <c r="AG13" s="15"/>
-      <c r="AH13" s="15"/>
-      <c r="AI13" s="15"/>
-      <c r="AJ13" s="15"/>
-      <c r="AK13" s="15"/>
-      <c r="AL13" s="18"/>
+      <c r="O13" s="27"/>
+      <c r="P13" s="27"/>
+      <c r="Q13" s="27"/>
+      <c r="R13" s="27"/>
+      <c r="S13" s="27"/>
+      <c r="T13" s="27"/>
+      <c r="U13" s="27"/>
+      <c r="V13" s="27"/>
+      <c r="W13" s="27"/>
+      <c r="X13" s="27"/>
+      <c r="Y13" s="29"/>
+      <c r="Z13" s="29"/>
+      <c r="AA13" s="29"/>
+      <c r="AB13" s="29"/>
+      <c r="AC13" s="29"/>
+      <c r="AD13" s="29"/>
+      <c r="AE13" s="29"/>
+      <c r="AF13" s="29"/>
+      <c r="AG13" s="29"/>
+      <c r="AH13" s="29"/>
+      <c r="AI13" s="29"/>
+      <c r="AJ13" s="29"/>
+      <c r="AK13" s="29"/>
+      <c r="AL13" s="29"/>
+      <c r="AM13" s="30"/>
     </row>
     <row r="14" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
+      <c r="B14" s="27">
+        <v>1</v>
+      </c>
+      <c r="C14" s="27"/>
       <c r="D14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14">
-        <v>1</v>
-      </c>
-      <c r="L14">
-        <v>1</v>
-      </c>
-      <c r="M14">
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27">
+        <v>1</v>
+      </c>
+      <c r="L14" s="27">
+        <v>1</v>
+      </c>
+      <c r="M14" s="27">
         <v>2</v>
       </c>
-      <c r="N14" s="1"/>
-      <c r="O14">
-        <v>3</v>
-      </c>
-      <c r="W14" s="3"/>
-      <c r="Y14" s="14"/>
-      <c r="Z14" s="15"/>
-      <c r="AA14" s="15"/>
-      <c r="AB14" s="15"/>
-      <c r="AC14" s="15"/>
-      <c r="AD14" s="15"/>
-      <c r="AE14" s="15"/>
-      <c r="AF14" s="15"/>
-      <c r="AG14" s="15"/>
-      <c r="AH14" s="15"/>
-      <c r="AI14" s="15"/>
-      <c r="AJ14" s="15"/>
-      <c r="AK14" s="15"/>
-      <c r="AL14" s="18"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="27">
+        <v>3</v>
+      </c>
+      <c r="P14" s="27"/>
+      <c r="Q14" s="27"/>
+      <c r="R14" s="27"/>
+      <c r="S14" s="27"/>
+      <c r="T14" s="27"/>
+      <c r="U14" s="27"/>
+      <c r="V14" s="27"/>
+      <c r="W14" s="27"/>
+      <c r="X14" s="27"/>
+      <c r="Y14" s="29"/>
+      <c r="Z14" s="29"/>
+      <c r="AA14" s="29"/>
+      <c r="AB14" s="29"/>
+      <c r="AC14" s="29"/>
+      <c r="AD14" s="29"/>
+      <c r="AE14" s="29"/>
+      <c r="AF14" s="29"/>
+      <c r="AG14" s="29"/>
+      <c r="AH14" s="29"/>
+      <c r="AI14" s="29"/>
+      <c r="AJ14" s="29"/>
+      <c r="AK14" s="29"/>
+      <c r="AL14" s="29"/>
+      <c r="AM14" s="30"/>
     </row>
     <row r="15" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
+      <c r="B15" s="27">
+        <v>1</v>
+      </c>
+      <c r="C15" s="27"/>
       <c r="D15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="L15">
-        <v>1</v>
-      </c>
-      <c r="N15">
-        <v>3</v>
-      </c>
-      <c r="O15" s="1"/>
-      <c r="P15">
-        <v>1</v>
-      </c>
-      <c r="W15" s="3"/>
-      <c r="Y15" s="14"/>
-      <c r="Z15" s="15"/>
-      <c r="AA15" s="15"/>
-      <c r="AB15" s="15"/>
-      <c r="AC15" s="15"/>
-      <c r="AD15" s="15"/>
-      <c r="AE15" s="15"/>
-      <c r="AF15" s="15"/>
-      <c r="AG15" s="15"/>
-      <c r="AH15" s="15"/>
-      <c r="AI15" s="15"/>
-      <c r="AJ15" s="15"/>
-      <c r="AK15" s="15"/>
-      <c r="AL15" s="18"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="27">
+        <v>1</v>
+      </c>
+      <c r="M15" s="27"/>
+      <c r="N15" s="27">
+        <v>3</v>
+      </c>
+      <c r="O15" s="28"/>
+      <c r="P15" s="27">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="27"/>
+      <c r="R15" s="27"/>
+      <c r="S15" s="27"/>
+      <c r="T15" s="27"/>
+      <c r="U15" s="27"/>
+      <c r="V15" s="27"/>
+      <c r="W15" s="27"/>
+      <c r="X15" s="27"/>
+      <c r="Y15" s="29"/>
+      <c r="Z15" s="29"/>
+      <c r="AA15" s="29"/>
+      <c r="AB15" s="29"/>
+      <c r="AC15" s="29"/>
+      <c r="AD15" s="29"/>
+      <c r="AE15" s="29"/>
+      <c r="AF15" s="29"/>
+      <c r="AG15" s="29"/>
+      <c r="AH15" s="29"/>
+      <c r="AI15" s="29"/>
+      <c r="AJ15" s="29"/>
+      <c r="AK15" s="29"/>
+      <c r="AL15" s="29"/>
+      <c r="AM15" s="30"/>
     </row>
     <row r="16" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16">
+      <c r="B16" s="27">
+        <v>1</v>
+      </c>
+      <c r="C16" s="27">
         <v>1</v>
       </c>
       <c r="D16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="L16">
-        <v>1</v>
-      </c>
-      <c r="O16">
-        <v>1</v>
-      </c>
-      <c r="P16" s="1"/>
-      <c r="R16">
-        <v>1</v>
-      </c>
-      <c r="T16">
-        <v>1</v>
-      </c>
-      <c r="W16" s="3"/>
-      <c r="X16">
-        <v>1</v>
-      </c>
-      <c r="Y16" s="14"/>
-      <c r="Z16" s="15"/>
-      <c r="AA16" s="15"/>
-      <c r="AB16" s="15"/>
-      <c r="AC16" s="15"/>
-      <c r="AD16" s="15"/>
-      <c r="AE16" s="15"/>
-      <c r="AF16" s="15"/>
-      <c r="AG16" s="15"/>
-      <c r="AH16" s="15"/>
-      <c r="AI16" s="15"/>
-      <c r="AJ16" s="15"/>
-      <c r="AK16" s="15"/>
-      <c r="AL16" s="18"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="27">
+        <v>1</v>
+      </c>
+      <c r="M16" s="27"/>
+      <c r="N16" s="27"/>
+      <c r="O16" s="27">
+        <v>1</v>
+      </c>
+      <c r="P16" s="28"/>
+      <c r="Q16" s="27"/>
+      <c r="R16" s="27">
+        <v>1</v>
+      </c>
+      <c r="S16" s="27"/>
+      <c r="T16" s="27">
+        <v>1</v>
+      </c>
+      <c r="U16" s="27"/>
+      <c r="V16" s="27"/>
+      <c r="W16" s="27"/>
+      <c r="X16" s="27">
+        <v>1</v>
+      </c>
+      <c r="Y16" s="29"/>
+      <c r="Z16" s="29"/>
+      <c r="AA16" s="29"/>
+      <c r="AB16" s="29"/>
+      <c r="AC16" s="29"/>
+      <c r="AD16" s="29"/>
+      <c r="AE16" s="29"/>
+      <c r="AF16" s="29"/>
+      <c r="AG16" s="29"/>
+      <c r="AH16" s="29"/>
+      <c r="AI16" s="29"/>
+      <c r="AJ16" s="29"/>
+      <c r="AK16" s="29"/>
+      <c r="AL16" s="29"/>
+      <c r="AM16" s="30"/>
     </row>
     <row r="17" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="C17">
+      <c r="B17" s="27"/>
+      <c r="C17" s="27">
         <v>1</v>
       </c>
       <c r="D17" s="8"/>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="J17" s="8"/>
-      <c r="L17">
-        <v>1</v>
-      </c>
-      <c r="Q17" s="1"/>
-      <c r="R17">
-        <v>1</v>
-      </c>
-      <c r="S17">
-        <v>1</v>
-      </c>
-      <c r="W17" s="3"/>
-      <c r="Y17" s="14"/>
-      <c r="Z17" s="15"/>
-      <c r="AA17" s="15"/>
-      <c r="AB17" s="15"/>
-      <c r="AC17" s="15"/>
-      <c r="AD17" s="15"/>
-      <c r="AE17" s="15"/>
-      <c r="AF17" s="15"/>
-      <c r="AG17" s="15"/>
-      <c r="AH17" s="15"/>
-      <c r="AI17" s="15"/>
-      <c r="AJ17" s="15"/>
-      <c r="AK17" s="15"/>
-      <c r="AL17" s="18"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27">
+        <v>1</v>
+      </c>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="27">
+        <v>1</v>
+      </c>
+      <c r="M17" s="27"/>
+      <c r="N17" s="27"/>
+      <c r="O17" s="27"/>
+      <c r="P17" s="27"/>
+      <c r="Q17" s="28"/>
+      <c r="R17" s="27">
+        <v>1</v>
+      </c>
+      <c r="S17" s="27">
+        <v>1</v>
+      </c>
+      <c r="T17" s="27"/>
+      <c r="U17" s="27"/>
+      <c r="V17" s="27"/>
+      <c r="W17" s="27"/>
+      <c r="X17" s="27"/>
+      <c r="Y17" s="29"/>
+      <c r="Z17" s="29"/>
+      <c r="AA17" s="29"/>
+      <c r="AB17" s="29"/>
+      <c r="AC17" s="29"/>
+      <c r="AD17" s="29"/>
+      <c r="AE17" s="29"/>
+      <c r="AF17" s="29"/>
+      <c r="AG17" s="29"/>
+      <c r="AH17" s="29"/>
+      <c r="AI17" s="29"/>
+      <c r="AJ17" s="29"/>
+      <c r="AK17" s="29"/>
+      <c r="AL17" s="29"/>
+      <c r="AM17" s="30"/>
     </row>
     <row r="18" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="C18">
+      <c r="B18" s="27"/>
+      <c r="C18" s="27">
         <v>1</v>
       </c>
       <c r="D18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="L18">
-        <v>1</v>
-      </c>
-      <c r="P18">
-        <v>1</v>
-      </c>
-      <c r="Q18">
-        <v>1</v>
-      </c>
-      <c r="R18" s="1"/>
-      <c r="W18" s="3"/>
-      <c r="Y18" s="14"/>
-      <c r="Z18" s="15"/>
-      <c r="AA18" s="15"/>
-      <c r="AB18" s="15"/>
-      <c r="AC18" s="15"/>
-      <c r="AD18" s="15"/>
-      <c r="AE18" s="15"/>
-      <c r="AF18" s="15"/>
-      <c r="AG18" s="15"/>
-      <c r="AH18" s="15"/>
-      <c r="AI18" s="15"/>
-      <c r="AJ18" s="15"/>
-      <c r="AK18" s="15"/>
-      <c r="AL18" s="18"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
+      <c r="L18" s="27">
+        <v>1</v>
+      </c>
+      <c r="M18" s="27"/>
+      <c r="N18" s="27"/>
+      <c r="O18" s="27"/>
+      <c r="P18" s="27">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="27">
+        <v>1</v>
+      </c>
+      <c r="R18" s="28"/>
+      <c r="S18" s="27"/>
+      <c r="T18" s="27"/>
+      <c r="U18" s="27"/>
+      <c r="V18" s="27"/>
+      <c r="W18" s="27"/>
+      <c r="X18" s="27"/>
+      <c r="Y18" s="29"/>
+      <c r="Z18" s="29"/>
+      <c r="AA18" s="29"/>
+      <c r="AB18" s="29"/>
+      <c r="AC18" s="29"/>
+      <c r="AD18" s="29"/>
+      <c r="AE18" s="29"/>
+      <c r="AF18" s="29"/>
+      <c r="AG18" s="29"/>
+      <c r="AH18" s="29"/>
+      <c r="AI18" s="29"/>
+      <c r="AJ18" s="29"/>
+      <c r="AK18" s="29"/>
+      <c r="AL18" s="29"/>
+      <c r="AM18" s="30"/>
     </row>
     <row r="19" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="C19">
+      <c r="B19" s="27"/>
+      <c r="C19" s="27">
         <v>1</v>
       </c>
       <c r="D19" s="8"/>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19">
-        <v>1</v>
-      </c>
-      <c r="J19" s="8"/>
-      <c r="Q19">
-        <v>1</v>
-      </c>
-      <c r="S19" s="1"/>
-      <c r="W19" s="3"/>
-      <c r="Y19" s="14"/>
-      <c r="Z19" s="15"/>
-      <c r="AA19" s="15"/>
-      <c r="AB19" s="15"/>
-      <c r="AC19" s="15"/>
-      <c r="AD19" s="15"/>
-      <c r="AE19" s="15"/>
-      <c r="AF19" s="15"/>
-      <c r="AG19" s="15"/>
-      <c r="AH19" s="15"/>
-      <c r="AI19" s="15"/>
-      <c r="AJ19" s="15"/>
-      <c r="AK19" s="15"/>
-      <c r="AL19" s="18"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27">
+        <v>1</v>
+      </c>
+      <c r="G19" s="27">
+        <v>1</v>
+      </c>
+      <c r="H19" s="27"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="27"/>
+      <c r="L19" s="27"/>
+      <c r="M19" s="27"/>
+      <c r="N19" s="27"/>
+      <c r="O19" s="27"/>
+      <c r="P19" s="27"/>
+      <c r="Q19" s="27">
+        <v>1</v>
+      </c>
+      <c r="R19" s="27"/>
+      <c r="S19" s="28"/>
+      <c r="T19" s="27"/>
+      <c r="U19" s="27"/>
+      <c r="V19" s="27"/>
+      <c r="W19" s="27"/>
+      <c r="X19" s="27"/>
+      <c r="Y19" s="29"/>
+      <c r="Z19" s="29"/>
+      <c r="AA19" s="29"/>
+      <c r="AB19" s="29"/>
+      <c r="AC19" s="29"/>
+      <c r="AD19" s="29"/>
+      <c r="AE19" s="29"/>
+      <c r="AF19" s="29"/>
+      <c r="AG19" s="29"/>
+      <c r="AH19" s="29"/>
+      <c r="AI19" s="29"/>
+      <c r="AJ19" s="29"/>
+      <c r="AK19" s="29"/>
+      <c r="AL19" s="29"/>
+      <c r="AM19" s="30"/>
     </row>
     <row r="20" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
+      <c r="B20" s="27">
+        <v>1</v>
+      </c>
+      <c r="C20" s="27"/>
       <c r="D20" s="8"/>
-      <c r="H20">
-        <v>1</v>
-      </c>
-      <c r="I20">
-        <v>1</v>
-      </c>
-      <c r="J20" s="8"/>
-      <c r="P20">
-        <v>1</v>
-      </c>
-      <c r="T20" s="1"/>
-      <c r="U20">
-        <v>1</v>
-      </c>
-      <c r="V20">
-        <v>1</v>
-      </c>
-      <c r="W20" s="3">
-        <v>1</v>
-      </c>
-      <c r="X20">
-        <v>1</v>
-      </c>
-      <c r="Y20" s="14"/>
-      <c r="Z20" s="15"/>
-      <c r="AA20" s="15"/>
-      <c r="AB20" s="15"/>
-      <c r="AC20" s="15"/>
-      <c r="AD20" s="15"/>
-      <c r="AE20" s="15"/>
-      <c r="AF20" s="15"/>
-      <c r="AG20" s="15"/>
-      <c r="AH20" s="15"/>
-      <c r="AI20" s="15"/>
-      <c r="AJ20" s="15"/>
-      <c r="AK20" s="15"/>
-      <c r="AL20" s="18"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27">
+        <v>1</v>
+      </c>
+      <c r="I20" s="3">
+        <v>1</v>
+      </c>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="27"/>
+      <c r="M20" s="27"/>
+      <c r="N20" s="27"/>
+      <c r="O20" s="27"/>
+      <c r="P20" s="27">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="27"/>
+      <c r="R20" s="27"/>
+      <c r="S20" s="27"/>
+      <c r="T20" s="28"/>
+      <c r="U20" s="27">
+        <v>1</v>
+      </c>
+      <c r="V20" s="27">
+        <v>1</v>
+      </c>
+      <c r="W20" s="27">
+        <v>1</v>
+      </c>
+      <c r="X20" s="27">
+        <v>1</v>
+      </c>
+      <c r="Y20" s="29"/>
+      <c r="Z20" s="29"/>
+      <c r="AA20" s="29"/>
+      <c r="AB20" s="29"/>
+      <c r="AC20" s="29"/>
+      <c r="AD20" s="29"/>
+      <c r="AE20" s="29"/>
+      <c r="AF20" s="29"/>
+      <c r="AG20" s="29"/>
+      <c r="AH20" s="29"/>
+      <c r="AI20" s="29"/>
+      <c r="AJ20" s="29"/>
+      <c r="AK20" s="29"/>
+      <c r="AL20" s="29"/>
+      <c r="AM20" s="30"/>
     </row>
     <row r="21" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="C21">
+      <c r="B21" s="27"/>
+      <c r="C21" s="27">
         <v>1</v>
       </c>
       <c r="D21" s="8"/>
-      <c r="I21">
-        <v>1</v>
-      </c>
-      <c r="J21" s="8"/>
-      <c r="T21">
-        <v>1</v>
-      </c>
-      <c r="U21" s="1"/>
-      <c r="V21">
-        <v>1</v>
-      </c>
-      <c r="W21" s="3"/>
-      <c r="Y21" s="14"/>
-      <c r="Z21" s="15"/>
-      <c r="AA21" s="15"/>
-      <c r="AB21" s="15"/>
-      <c r="AC21" s="15"/>
-      <c r="AD21" s="15"/>
-      <c r="AE21" s="15"/>
-      <c r="AF21" s="15"/>
-      <c r="AG21" s="15"/>
-      <c r="AH21" s="15"/>
-      <c r="AI21" s="15"/>
-      <c r="AJ21" s="15"/>
-      <c r="AK21" s="15"/>
-      <c r="AL21" s="18"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="3">
+        <v>1</v>
+      </c>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="27"/>
+      <c r="M21" s="27"/>
+      <c r="N21" s="27"/>
+      <c r="O21" s="27"/>
+      <c r="P21" s="27"/>
+      <c r="Q21" s="27"/>
+      <c r="R21" s="27"/>
+      <c r="S21" s="27"/>
+      <c r="T21" s="27">
+        <v>1</v>
+      </c>
+      <c r="U21" s="28"/>
+      <c r="V21" s="27">
+        <v>1</v>
+      </c>
+      <c r="W21" s="27"/>
+      <c r="X21" s="27"/>
+      <c r="Y21" s="29"/>
+      <c r="Z21" s="29"/>
+      <c r="AA21" s="29"/>
+      <c r="AB21" s="29"/>
+      <c r="AC21" s="29"/>
+      <c r="AD21" s="29"/>
+      <c r="AE21" s="29"/>
+      <c r="AF21" s="29"/>
+      <c r="AG21" s="29"/>
+      <c r="AH21" s="29"/>
+      <c r="AI21" s="29"/>
+      <c r="AJ21" s="29"/>
+      <c r="AK21" s="29"/>
+      <c r="AL21" s="29"/>
+      <c r="AM21" s="30"/>
     </row>
     <row r="22" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="C22">
+      <c r="B22" s="27"/>
+      <c r="C22" s="27">
         <v>1</v>
       </c>
       <c r="D22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="T22">
-        <v>1</v>
-      </c>
-      <c r="U22">
-        <v>1</v>
-      </c>
-      <c r="V22" s="1"/>
-      <c r="W22" s="2">
-        <v>1</v>
-      </c>
-      <c r="Y22" s="14"/>
-      <c r="Z22" s="15"/>
-      <c r="AA22" s="15"/>
-      <c r="AB22" s="15"/>
-      <c r="AC22" s="15"/>
-      <c r="AD22" s="15"/>
-      <c r="AE22" s="15"/>
-      <c r="AF22" s="15"/>
-      <c r="AG22" s="15"/>
-      <c r="AH22" s="15"/>
-      <c r="AI22" s="15"/>
-      <c r="AJ22" s="15"/>
-      <c r="AK22" s="15"/>
-      <c r="AL22" s="18"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="27"/>
+      <c r="M22" s="27"/>
+      <c r="N22" s="27"/>
+      <c r="O22" s="27"/>
+      <c r="P22" s="27"/>
+      <c r="Q22" s="27"/>
+      <c r="R22" s="27"/>
+      <c r="S22" s="27"/>
+      <c r="T22" s="27">
+        <v>1</v>
+      </c>
+      <c r="U22" s="27">
+        <v>1</v>
+      </c>
+      <c r="V22" s="28"/>
+      <c r="W22" s="27">
+        <v>1</v>
+      </c>
+      <c r="X22" s="27"/>
+      <c r="Y22" s="29"/>
+      <c r="Z22" s="29"/>
+      <c r="AA22" s="29"/>
+      <c r="AB22" s="29"/>
+      <c r="AC22" s="29"/>
+      <c r="AD22" s="29"/>
+      <c r="AE22" s="29"/>
+      <c r="AF22" s="29"/>
+      <c r="AG22" s="29"/>
+      <c r="AH22" s="29"/>
+      <c r="AI22" s="29"/>
+      <c r="AJ22" s="29"/>
+      <c r="AK22" s="29"/>
+      <c r="AL22" s="29"/>
+      <c r="AM22" s="30"/>
     </row>
     <row r="23" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="D23" s="9"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-      <c r="O23" s="2"/>
-      <c r="P23" s="2"/>
-      <c r="Q23" s="2"/>
-      <c r="R23" s="2"/>
-      <c r="S23" s="2"/>
-      <c r="T23" s="2">
-        <v>1</v>
-      </c>
-      <c r="U23" s="2"/>
-      <c r="V23" s="2">
-        <v>1</v>
-      </c>
-      <c r="W23" s="10"/>
-      <c r="X23" s="2">
-        <v>1</v>
-      </c>
-      <c r="Y23" s="20"/>
-      <c r="Z23" s="21"/>
-      <c r="AA23" s="21"/>
-      <c r="AB23" s="21"/>
-      <c r="AC23" s="21"/>
-      <c r="AD23" s="21"/>
-      <c r="AE23" s="21"/>
-      <c r="AF23" s="21"/>
-      <c r="AG23" s="21"/>
-      <c r="AH23" s="21"/>
-      <c r="AI23" s="21"/>
-      <c r="AJ23" s="21"/>
-      <c r="AK23" s="21"/>
-      <c r="AL23" s="22"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="27">
+        <v>1</v>
+      </c>
+      <c r="D23" s="8"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="27"/>
+      <c r="M23" s="27"/>
+      <c r="N23" s="27"/>
+      <c r="O23" s="27"/>
+      <c r="P23" s="27"/>
+      <c r="Q23" s="27"/>
+      <c r="R23" s="27"/>
+      <c r="S23" s="27"/>
+      <c r="T23" s="27">
+        <v>1</v>
+      </c>
+      <c r="U23" s="27"/>
+      <c r="V23" s="27">
+        <v>1</v>
+      </c>
+      <c r="W23" s="28"/>
+      <c r="X23" s="27">
+        <v>1</v>
+      </c>
+      <c r="Y23" s="29"/>
+      <c r="Z23" s="29"/>
+      <c r="AA23" s="29"/>
+      <c r="AB23" s="29"/>
+      <c r="AC23" s="29"/>
+      <c r="AD23" s="29"/>
+      <c r="AE23" s="29"/>
+      <c r="AF23" s="29"/>
+      <c r="AG23" s="29"/>
+      <c r="AH23" s="29"/>
+      <c r="AI23" s="29"/>
+      <c r="AJ23" s="29"/>
+      <c r="AK23" s="29"/>
+      <c r="AL23" s="29"/>
+      <c r="AM23" s="30"/>
     </row>
     <row r="24" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="P24">
-        <v>1</v>
-      </c>
-      <c r="T24">
-        <v>1</v>
-      </c>
-      <c r="W24" s="3">
-        <v>1</v>
-      </c>
-      <c r="X24" s="1"/>
-      <c r="Y24" s="14"/>
-      <c r="Z24" s="15"/>
-      <c r="AA24" s="15"/>
-      <c r="AB24" s="15"/>
-      <c r="AC24" s="15"/>
-      <c r="AD24" s="15"/>
-      <c r="AE24" s="15"/>
-      <c r="AF24" s="15"/>
-      <c r="AG24" s="15"/>
-      <c r="AH24" s="15"/>
-      <c r="AI24" s="15"/>
-      <c r="AJ24" s="15"/>
-      <c r="AK24" s="15"/>
-      <c r="AL24" s="18"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="27">
+        <v>1</v>
+      </c>
+      <c r="D24" s="9"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="27"/>
+      <c r="L24" s="27"/>
+      <c r="M24" s="27"/>
+      <c r="N24" s="27"/>
+      <c r="O24" s="27"/>
+      <c r="P24" s="27">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="27"/>
+      <c r="R24" s="27"/>
+      <c r="S24" s="27"/>
+      <c r="T24" s="27">
+        <v>1</v>
+      </c>
+      <c r="U24" s="27"/>
+      <c r="V24" s="27"/>
+      <c r="W24" s="27">
+        <v>1</v>
+      </c>
+      <c r="X24" s="28"/>
+      <c r="Y24" s="29"/>
+      <c r="Z24" s="29"/>
+      <c r="AA24" s="29"/>
+      <c r="AB24" s="29"/>
+      <c r="AC24" s="29"/>
+      <c r="AD24" s="29"/>
+      <c r="AE24" s="29"/>
+      <c r="AF24" s="29"/>
+      <c r="AG24" s="29"/>
+      <c r="AH24" s="29"/>
+      <c r="AI24" s="29"/>
+      <c r="AJ24" s="29"/>
+      <c r="AK24" s="29"/>
+      <c r="AL24" s="29"/>
+      <c r="AM24" s="30"/>
     </row>
     <row r="25" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="27" t="s">
         <v>16</v>
       </c>
+      <c r="B25" s="27"/>
+      <c r="C25" s="27"/>
       <c r="D25" s="8">
         <v>3</v>
       </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
-      <c r="J25" s="12">
-        <v>3</v>
-      </c>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="13"/>
-      <c r="N25" s="13"/>
-      <c r="O25" s="13"/>
-      <c r="P25" s="13"/>
-      <c r="Q25" s="13"/>
-      <c r="R25" s="13"/>
-      <c r="S25" s="13"/>
-      <c r="T25" s="13"/>
-      <c r="U25" s="13"/>
-      <c r="V25" s="13"/>
-      <c r="W25" s="16"/>
-      <c r="X25" s="15"/>
-      <c r="Y25" s="17"/>
-      <c r="Z25" s="8">
-        <v>3</v>
-      </c>
-      <c r="AB25">
-        <v>3</v>
-      </c>
-      <c r="AL25" s="3"/>
+      <c r="E25" s="27">
+        <v>1</v>
+      </c>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="29">
+        <v>3</v>
+      </c>
+      <c r="K25" s="29"/>
+      <c r="L25" s="29"/>
+      <c r="M25" s="29"/>
+      <c r="N25" s="29"/>
+      <c r="O25" s="29"/>
+      <c r="P25" s="29"/>
+      <c r="Q25" s="29"/>
+      <c r="R25" s="29"/>
+      <c r="S25" s="29"/>
+      <c r="T25" s="29"/>
+      <c r="U25" s="29"/>
+      <c r="V25" s="29"/>
+      <c r="W25" s="29"/>
+      <c r="X25" s="29"/>
+      <c r="Y25" s="28"/>
+      <c r="Z25" s="27">
+        <v>3</v>
+      </c>
+      <c r="AA25" s="27"/>
+      <c r="AB25" s="27">
+        <v>3</v>
+      </c>
+      <c r="AC25" s="27"/>
+      <c r="AD25" s="27"/>
+      <c r="AE25" s="27"/>
+      <c r="AF25" s="27"/>
+      <c r="AG25" s="27"/>
+      <c r="AH25" s="27"/>
+      <c r="AI25" s="27"/>
+      <c r="AJ25" s="27"/>
+      <c r="AK25" s="27"/>
+      <c r="AL25" s="27"/>
+      <c r="AM25" s="27"/>
     </row>
     <row r="26" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="27" t="s">
         <v>17</v>
       </c>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
       <c r="D26" s="8"/>
-      <c r="E26">
-        <v>1</v>
-      </c>
-      <c r="J26" s="14"/>
-      <c r="K26" s="15"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="15"/>
-      <c r="N26" s="15"/>
-      <c r="O26" s="15"/>
-      <c r="P26" s="15"/>
-      <c r="Q26" s="15"/>
-      <c r="R26" s="15"/>
-      <c r="S26" s="15"/>
-      <c r="T26" s="15"/>
-      <c r="U26" s="15"/>
-      <c r="V26" s="15"/>
-      <c r="W26" s="18"/>
-      <c r="X26" s="15"/>
-      <c r="Y26" s="8">
-        <v>3</v>
-      </c>
-      <c r="Z26" s="1"/>
-      <c r="AA26">
-        <v>1</v>
-      </c>
-      <c r="AB26">
-        <v>3</v>
-      </c>
-      <c r="AC26">
-        <v>1</v>
-      </c>
-      <c r="AL26" s="3"/>
+      <c r="E26" s="27">
+        <v>1</v>
+      </c>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="29"/>
+      <c r="K26" s="29"/>
+      <c r="L26" s="29"/>
+      <c r="M26" s="29"/>
+      <c r="N26" s="29"/>
+      <c r="O26" s="29"/>
+      <c r="P26" s="29"/>
+      <c r="Q26" s="29"/>
+      <c r="R26" s="29"/>
+      <c r="S26" s="29"/>
+      <c r="T26" s="29"/>
+      <c r="U26" s="29"/>
+      <c r="V26" s="29"/>
+      <c r="W26" s="29"/>
+      <c r="X26" s="29"/>
+      <c r="Y26" s="27">
+        <v>3</v>
+      </c>
+      <c r="Z26" s="28"/>
+      <c r="AA26" s="27">
+        <v>1</v>
+      </c>
+      <c r="AB26" s="27">
+        <v>3</v>
+      </c>
+      <c r="AC26" s="27">
+        <v>1</v>
+      </c>
+      <c r="AD26" s="27"/>
+      <c r="AE26" s="27"/>
+      <c r="AF26" s="27"/>
+      <c r="AG26" s="27"/>
+      <c r="AH26" s="27"/>
+      <c r="AI26" s="27"/>
+      <c r="AJ26" s="27"/>
+      <c r="AK26" s="27"/>
+      <c r="AL26" s="27"/>
+      <c r="AM26" s="27"/>
     </row>
     <row r="27" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="27" t="s">
         <v>18</v>
       </c>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
       <c r="D27" s="8"/>
-      <c r="E27">
-        <v>1</v>
-      </c>
-      <c r="F27">
-        <v>1</v>
-      </c>
-      <c r="J27" s="14"/>
-      <c r="K27" s="15"/>
-      <c r="L27" s="15"/>
-      <c r="M27" s="15"/>
-      <c r="N27" s="15"/>
-      <c r="O27" s="15"/>
-      <c r="P27" s="15"/>
-      <c r="Q27" s="15"/>
-      <c r="R27" s="15"/>
-      <c r="S27" s="15"/>
-      <c r="T27" s="15"/>
-      <c r="U27" s="15"/>
-      <c r="V27" s="15"/>
-      <c r="W27" s="18"/>
-      <c r="X27" s="15"/>
-      <c r="Y27" s="8"/>
-      <c r="Z27">
-        <v>1</v>
-      </c>
-      <c r="AA27" s="1"/>
-      <c r="AC27">
-        <v>1</v>
-      </c>
-      <c r="AD27">
-        <v>1</v>
-      </c>
-      <c r="AE27">
-        <v>1</v>
-      </c>
-      <c r="AF27">
-        <v>1</v>
-      </c>
-      <c r="AG27">
-        <v>1</v>
-      </c>
-      <c r="AL27" s="3"/>
+      <c r="E27" s="27">
+        <v>1</v>
+      </c>
+      <c r="F27" s="27">
+        <v>1</v>
+      </c>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="29"/>
+      <c r="K27" s="29"/>
+      <c r="L27" s="29"/>
+      <c r="M27" s="29"/>
+      <c r="N27" s="29"/>
+      <c r="O27" s="29"/>
+      <c r="P27" s="29"/>
+      <c r="Q27" s="29"/>
+      <c r="R27" s="29"/>
+      <c r="S27" s="29"/>
+      <c r="T27" s="29"/>
+      <c r="U27" s="29"/>
+      <c r="V27" s="29"/>
+      <c r="W27" s="29"/>
+      <c r="X27" s="29"/>
+      <c r="Y27" s="27"/>
+      <c r="Z27" s="27">
+        <v>1</v>
+      </c>
+      <c r="AA27" s="28"/>
+      <c r="AB27" s="27"/>
+      <c r="AC27" s="27">
+        <v>1</v>
+      </c>
+      <c r="AD27" s="27">
+        <v>1</v>
+      </c>
+      <c r="AE27" s="27">
+        <v>1</v>
+      </c>
+      <c r="AF27" s="27">
+        <v>1</v>
+      </c>
+      <c r="AG27" s="27">
+        <v>1</v>
+      </c>
+      <c r="AH27" s="27"/>
+      <c r="AI27" s="27"/>
+      <c r="AJ27" s="27"/>
+      <c r="AK27" s="27"/>
+      <c r="AL27" s="27"/>
+      <c r="AM27" s="27"/>
     </row>
     <row r="28" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
+      <c r="B28" s="27">
+        <v>1</v>
+      </c>
+      <c r="C28" s="27"/>
       <c r="D28" s="8">
         <v>3</v>
       </c>
-      <c r="J28" s="14"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="15"/>
-      <c r="N28" s="15"/>
-      <c r="O28" s="15"/>
-      <c r="P28" s="15"/>
-      <c r="Q28" s="15"/>
-      <c r="R28" s="15"/>
-      <c r="S28" s="15"/>
-      <c r="T28" s="15"/>
-      <c r="U28" s="15"/>
-      <c r="V28" s="15"/>
-      <c r="W28" s="18"/>
-      <c r="X28" s="15"/>
-      <c r="Y28" s="8">
-        <v>3</v>
-      </c>
-      <c r="Z28">
-        <v>3</v>
-      </c>
-      <c r="AB28" s="1"/>
-      <c r="AC28">
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="29"/>
+      <c r="K28" s="29"/>
+      <c r="L28" s="29"/>
+      <c r="M28" s="29"/>
+      <c r="N28" s="29"/>
+      <c r="O28" s="29"/>
+      <c r="P28" s="29"/>
+      <c r="Q28" s="29"/>
+      <c r="R28" s="29"/>
+      <c r="S28" s="29"/>
+      <c r="T28" s="29"/>
+      <c r="U28" s="29"/>
+      <c r="V28" s="29"/>
+      <c r="W28" s="29"/>
+      <c r="X28" s="29"/>
+      <c r="Y28" s="27">
+        <v>3</v>
+      </c>
+      <c r="Z28" s="27">
+        <v>3</v>
+      </c>
+      <c r="AA28" s="27"/>
+      <c r="AB28" s="28"/>
+      <c r="AC28" s="27">
         <v>2</v>
       </c>
-      <c r="AL28" s="3"/>
+      <c r="AD28" s="27"/>
+      <c r="AE28" s="27"/>
+      <c r="AF28" s="27"/>
+      <c r="AG28" s="27"/>
+      <c r="AH28" s="27"/>
+      <c r="AI28" s="27"/>
+      <c r="AJ28" s="27"/>
+      <c r="AK28" s="27"/>
+      <c r="AL28" s="27"/>
+      <c r="AM28" s="27"/>
     </row>
     <row r="29" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
+      <c r="B29" s="27">
+        <v>1</v>
+      </c>
+      <c r="C29" s="27"/>
       <c r="D29" s="8"/>
-      <c r="J29" s="14"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="15"/>
-      <c r="M29" s="15"/>
-      <c r="N29" s="15"/>
-      <c r="O29" s="15"/>
-      <c r="P29" s="15"/>
-      <c r="Q29" s="15"/>
-      <c r="R29" s="15"/>
-      <c r="S29" s="15"/>
-      <c r="T29" s="15"/>
-      <c r="U29" s="15"/>
-      <c r="V29" s="15"/>
-      <c r="W29" s="18"/>
-      <c r="X29" s="15"/>
-      <c r="Y29" s="8"/>
-      <c r="Z29">
-        <v>1</v>
-      </c>
-      <c r="AA29">
-        <v>1</v>
-      </c>
-      <c r="AB29">
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="29"/>
+      <c r="K29" s="29"/>
+      <c r="L29" s="29"/>
+      <c r="M29" s="29"/>
+      <c r="N29" s="29"/>
+      <c r="O29" s="29"/>
+      <c r="P29" s="29"/>
+      <c r="Q29" s="29"/>
+      <c r="R29" s="29"/>
+      <c r="S29" s="29"/>
+      <c r="T29" s="29"/>
+      <c r="U29" s="29"/>
+      <c r="V29" s="29"/>
+      <c r="W29" s="29"/>
+      <c r="X29" s="29"/>
+      <c r="Y29" s="27"/>
+      <c r="Z29" s="27">
+        <v>1</v>
+      </c>
+      <c r="AA29" s="27">
+        <v>1</v>
+      </c>
+      <c r="AB29" s="27">
         <v>2</v>
       </c>
-      <c r="AC29" s="1"/>
-      <c r="AD29">
-        <v>3</v>
-      </c>
-      <c r="AL29" s="3"/>
+      <c r="AC29" s="28"/>
+      <c r="AD29" s="27">
+        <v>3</v>
+      </c>
+      <c r="AE29" s="27"/>
+      <c r="AF29" s="27"/>
+      <c r="AG29" s="27"/>
+      <c r="AH29" s="27"/>
+      <c r="AI29" s="27"/>
+      <c r="AJ29" s="27"/>
+      <c r="AK29" s="27"/>
+      <c r="AL29" s="27"/>
+      <c r="AM29" s="27"/>
     </row>
     <row r="30" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
+      <c r="B30" s="27">
+        <v>1</v>
+      </c>
+      <c r="C30" s="27"/>
       <c r="D30" s="8"/>
-      <c r="J30" s="14"/>
-      <c r="K30" s="15"/>
-      <c r="L30" s="15"/>
-      <c r="M30" s="15"/>
-      <c r="N30" s="15"/>
-      <c r="O30" s="15"/>
-      <c r="P30" s="15"/>
-      <c r="Q30" s="15"/>
-      <c r="R30" s="15"/>
-      <c r="S30" s="15"/>
-      <c r="T30" s="15"/>
-      <c r="U30" s="15"/>
-      <c r="V30" s="15"/>
-      <c r="W30" s="18"/>
-      <c r="X30" s="15"/>
-      <c r="Y30" s="8"/>
-      <c r="AA30">
-        <v>1</v>
-      </c>
-      <c r="AC30">
-        <v>3</v>
-      </c>
-      <c r="AD30" s="1"/>
-      <c r="AE30">
-        <v>1</v>
-      </c>
-      <c r="AL30" s="3"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="29"/>
+      <c r="K30" s="29"/>
+      <c r="L30" s="29"/>
+      <c r="M30" s="29"/>
+      <c r="N30" s="29"/>
+      <c r="O30" s="29"/>
+      <c r="P30" s="29"/>
+      <c r="Q30" s="29"/>
+      <c r="R30" s="29"/>
+      <c r="S30" s="29"/>
+      <c r="T30" s="29"/>
+      <c r="U30" s="29"/>
+      <c r="V30" s="29"/>
+      <c r="W30" s="29"/>
+      <c r="X30" s="29"/>
+      <c r="Y30" s="27"/>
+      <c r="Z30" s="27"/>
+      <c r="AA30" s="27">
+        <v>1</v>
+      </c>
+      <c r="AB30" s="27"/>
+      <c r="AC30" s="27">
+        <v>3</v>
+      </c>
+      <c r="AD30" s="28"/>
+      <c r="AE30" s="27">
+        <v>1</v>
+      </c>
+      <c r="AF30" s="27"/>
+      <c r="AG30" s="27"/>
+      <c r="AH30" s="27"/>
+      <c r="AI30" s="27"/>
+      <c r="AJ30" s="27"/>
+      <c r="AK30" s="27"/>
+      <c r="AL30" s="27"/>
+      <c r="AM30" s="27"/>
     </row>
     <row r="31" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31">
+      <c r="B31" s="27">
+        <v>1</v>
+      </c>
+      <c r="C31" s="27">
         <v>1</v>
       </c>
       <c r="D31" s="8"/>
-      <c r="J31" s="14"/>
-      <c r="K31" s="15"/>
-      <c r="L31" s="15"/>
-      <c r="M31" s="15"/>
-      <c r="N31" s="15"/>
-      <c r="O31" s="15"/>
-      <c r="P31" s="15"/>
-      <c r="Q31" s="15"/>
-      <c r="R31" s="15"/>
-      <c r="S31" s="15"/>
-      <c r="T31" s="15"/>
-      <c r="U31" s="15"/>
-      <c r="V31" s="15"/>
-      <c r="W31" s="18"/>
-      <c r="X31" s="15"/>
-      <c r="Y31" s="8"/>
-      <c r="AA31">
-        <v>1</v>
-      </c>
-      <c r="AD31">
-        <v>1</v>
-      </c>
-      <c r="AE31" s="1"/>
-      <c r="AG31">
-        <v>1</v>
-      </c>
-      <c r="AI31">
-        <v>1</v>
-      </c>
-      <c r="AL31" s="3"/>
-      <c r="AM31">
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="29"/>
+      <c r="K31" s="29"/>
+      <c r="L31" s="29"/>
+      <c r="M31" s="29"/>
+      <c r="N31" s="29"/>
+      <c r="O31" s="29"/>
+      <c r="P31" s="29"/>
+      <c r="Q31" s="29"/>
+      <c r="R31" s="29"/>
+      <c r="S31" s="29"/>
+      <c r="T31" s="29"/>
+      <c r="U31" s="29"/>
+      <c r="V31" s="29"/>
+      <c r="W31" s="29"/>
+      <c r="X31" s="29"/>
+      <c r="Y31" s="27"/>
+      <c r="Z31" s="27"/>
+      <c r="AA31" s="27">
+        <v>1</v>
+      </c>
+      <c r="AB31" s="27"/>
+      <c r="AC31" s="27"/>
+      <c r="AD31" s="27">
+        <v>1</v>
+      </c>
+      <c r="AE31" s="28"/>
+      <c r="AF31" s="27"/>
+      <c r="AG31" s="27">
+        <v>1</v>
+      </c>
+      <c r="AH31" s="27"/>
+      <c r="AI31" s="27">
+        <v>1</v>
+      </c>
+      <c r="AJ31" s="27"/>
+      <c r="AK31" s="27"/>
+      <c r="AL31" s="27"/>
+      <c r="AM31" s="27">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="C32">
+      <c r="B32" s="27"/>
+      <c r="C32" s="27">
         <v>1</v>
       </c>
       <c r="D32" s="8"/>
-      <c r="F32">
-        <v>1</v>
-      </c>
-      <c r="J32" s="14"/>
-      <c r="K32" s="15"/>
-      <c r="L32" s="15"/>
-      <c r="M32" s="15"/>
-      <c r="N32" s="15"/>
-      <c r="O32" s="15"/>
-      <c r="P32" s="15"/>
-      <c r="Q32" s="15"/>
-      <c r="R32" s="15"/>
-      <c r="S32" s="15"/>
-      <c r="T32" s="15"/>
-      <c r="U32" s="15"/>
-      <c r="V32" s="15"/>
-      <c r="W32" s="18"/>
-      <c r="X32" s="15"/>
-      <c r="Y32" s="8"/>
-      <c r="AA32">
-        <v>1</v>
-      </c>
-      <c r="AF32" s="1"/>
-      <c r="AG32">
-        <v>1</v>
-      </c>
-      <c r="AH32">
-        <v>1</v>
-      </c>
-      <c r="AL32" s="3"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27">
+        <v>1</v>
+      </c>
+      <c r="G32" s="27"/>
+      <c r="H32" s="27"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="29"/>
+      <c r="K32" s="29"/>
+      <c r="L32" s="29"/>
+      <c r="M32" s="29"/>
+      <c r="N32" s="29"/>
+      <c r="O32" s="29"/>
+      <c r="P32" s="29"/>
+      <c r="Q32" s="29"/>
+      <c r="R32" s="29"/>
+      <c r="S32" s="29"/>
+      <c r="T32" s="29"/>
+      <c r="U32" s="29"/>
+      <c r="V32" s="29"/>
+      <c r="W32" s="29"/>
+      <c r="X32" s="29"/>
+      <c r="Y32" s="27"/>
+      <c r="Z32" s="27"/>
+      <c r="AA32" s="27">
+        <v>1</v>
+      </c>
+      <c r="AB32" s="27"/>
+      <c r="AC32" s="27"/>
+      <c r="AD32" s="27"/>
+      <c r="AE32" s="27"/>
+      <c r="AF32" s="28"/>
+      <c r="AG32" s="27">
+        <v>1</v>
+      </c>
+      <c r="AH32" s="27">
+        <v>1</v>
+      </c>
+      <c r="AI32" s="27"/>
+      <c r="AJ32" s="27"/>
+      <c r="AK32" s="27"/>
+      <c r="AL32" s="27"/>
+      <c r="AM32" s="27"/>
     </row>
     <row r="33" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="A33" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="C33">
+      <c r="B33" s="27"/>
+      <c r="C33" s="27">
         <v>1</v>
       </c>
       <c r="D33" s="8"/>
-      <c r="J33" s="14"/>
-      <c r="K33" s="15"/>
-      <c r="L33" s="15"/>
-      <c r="M33" s="15"/>
-      <c r="N33" s="15"/>
-      <c r="O33" s="15"/>
-      <c r="P33" s="15"/>
-      <c r="Q33" s="15"/>
-      <c r="R33" s="15"/>
-      <c r="S33" s="15"/>
-      <c r="T33" s="15"/>
-      <c r="U33" s="15"/>
-      <c r="V33" s="15"/>
-      <c r="W33" s="18"/>
-      <c r="X33" s="15"/>
-      <c r="Y33" s="8"/>
-      <c r="AA33">
-        <v>1</v>
-      </c>
-      <c r="AE33">
-        <v>1</v>
-      </c>
-      <c r="AF33">
-        <v>1</v>
-      </c>
-      <c r="AG33" s="1"/>
-      <c r="AL33" s="3"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="27"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="29"/>
+      <c r="K33" s="29"/>
+      <c r="L33" s="29"/>
+      <c r="M33" s="29"/>
+      <c r="N33" s="29"/>
+      <c r="O33" s="29"/>
+      <c r="P33" s="29"/>
+      <c r="Q33" s="29"/>
+      <c r="R33" s="29"/>
+      <c r="S33" s="29"/>
+      <c r="T33" s="29"/>
+      <c r="U33" s="29"/>
+      <c r="V33" s="29"/>
+      <c r="W33" s="29"/>
+      <c r="X33" s="29"/>
+      <c r="Y33" s="27"/>
+      <c r="Z33" s="27"/>
+      <c r="AA33" s="27">
+        <v>1</v>
+      </c>
+      <c r="AB33" s="27"/>
+      <c r="AC33" s="27"/>
+      <c r="AD33" s="27"/>
+      <c r="AE33" s="27">
+        <v>1</v>
+      </c>
+      <c r="AF33" s="27">
+        <v>1</v>
+      </c>
+      <c r="AG33" s="28"/>
+      <c r="AH33" s="27"/>
+      <c r="AI33" s="27"/>
+      <c r="AJ33" s="27"/>
+      <c r="AK33" s="27"/>
+      <c r="AL33" s="27"/>
+      <c r="AM33" s="27"/>
     </row>
     <row r="34" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="A34" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="C34">
+      <c r="B34" s="27"/>
+      <c r="C34" s="27">
         <v>1</v>
       </c>
       <c r="D34" s="8"/>
-      <c r="F34">
-        <v>1</v>
-      </c>
-      <c r="G34">
-        <v>1</v>
-      </c>
-      <c r="J34" s="14"/>
-      <c r="K34" s="15"/>
-      <c r="L34" s="15"/>
-      <c r="M34" s="15"/>
-      <c r="N34" s="15"/>
-      <c r="O34" s="15"/>
-      <c r="P34" s="15"/>
-      <c r="Q34" s="15"/>
-      <c r="R34" s="15"/>
-      <c r="S34" s="15"/>
-      <c r="T34" s="15"/>
-      <c r="U34" s="15"/>
-      <c r="V34" s="15"/>
-      <c r="W34" s="18"/>
-      <c r="X34" s="15"/>
-      <c r="Y34" s="8"/>
-      <c r="AF34">
-        <v>1</v>
-      </c>
-      <c r="AH34" s="1"/>
-      <c r="AL34" s="3"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="27">
+        <v>1</v>
+      </c>
+      <c r="G34" s="27">
+        <v>1</v>
+      </c>
+      <c r="H34" s="27"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="29"/>
+      <c r="K34" s="29"/>
+      <c r="L34" s="29"/>
+      <c r="M34" s="29"/>
+      <c r="N34" s="29"/>
+      <c r="O34" s="29"/>
+      <c r="P34" s="29"/>
+      <c r="Q34" s="29"/>
+      <c r="R34" s="29"/>
+      <c r="S34" s="29"/>
+      <c r="T34" s="29"/>
+      <c r="U34" s="29"/>
+      <c r="V34" s="29"/>
+      <c r="W34" s="29"/>
+      <c r="X34" s="29"/>
+      <c r="Y34" s="27"/>
+      <c r="Z34" s="27"/>
+      <c r="AA34" s="27"/>
+      <c r="AB34" s="27"/>
+      <c r="AC34" s="27"/>
+      <c r="AD34" s="27"/>
+      <c r="AE34" s="27"/>
+      <c r="AF34" s="27">
+        <v>1</v>
+      </c>
+      <c r="AG34" s="27"/>
+      <c r="AH34" s="28"/>
+      <c r="AI34" s="27"/>
+      <c r="AJ34" s="27"/>
+      <c r="AK34" s="27"/>
+      <c r="AL34" s="27"/>
+      <c r="AM34" s="27"/>
     </row>
     <row r="35" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="A35" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
+      <c r="B35" s="27">
+        <v>1</v>
+      </c>
+      <c r="C35" s="27"/>
       <c r="D35" s="8"/>
-      <c r="H35">
-        <v>1</v>
-      </c>
-      <c r="I35">
-        <v>1</v>
-      </c>
-      <c r="J35" s="14"/>
-      <c r="K35" s="15"/>
-      <c r="L35" s="15"/>
-      <c r="M35" s="15"/>
-      <c r="N35" s="15"/>
-      <c r="O35" s="15"/>
-      <c r="P35" s="15"/>
-      <c r="Q35" s="15"/>
-      <c r="R35" s="15"/>
-      <c r="S35" s="15"/>
-      <c r="T35" s="15"/>
-      <c r="U35" s="15"/>
-      <c r="V35" s="15"/>
-      <c r="W35" s="18"/>
-      <c r="X35" s="15"/>
-      <c r="Y35" s="8"/>
-      <c r="AE35">
-        <v>1</v>
-      </c>
-      <c r="AI35" s="1"/>
-      <c r="AJ35">
-        <v>1</v>
-      </c>
-      <c r="AK35">
-        <v>1</v>
-      </c>
-      <c r="AL35" s="3">
-        <v>1</v>
-      </c>
-      <c r="AM35">
+      <c r="E35" s="27"/>
+      <c r="F35" s="27"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="27">
+        <v>1</v>
+      </c>
+      <c r="I35" s="3">
+        <v>1</v>
+      </c>
+      <c r="J35" s="29"/>
+      <c r="K35" s="29"/>
+      <c r="L35" s="29"/>
+      <c r="M35" s="29"/>
+      <c r="N35" s="29"/>
+      <c r="O35" s="29"/>
+      <c r="P35" s="29"/>
+      <c r="Q35" s="29"/>
+      <c r="R35" s="29"/>
+      <c r="S35" s="29"/>
+      <c r="T35" s="29"/>
+      <c r="U35" s="29"/>
+      <c r="V35" s="29"/>
+      <c r="W35" s="29"/>
+      <c r="X35" s="29"/>
+      <c r="Y35" s="27"/>
+      <c r="Z35" s="27"/>
+      <c r="AA35" s="27"/>
+      <c r="AB35" s="27"/>
+      <c r="AC35" s="27"/>
+      <c r="AD35" s="27"/>
+      <c r="AE35" s="27">
+        <v>1</v>
+      </c>
+      <c r="AF35" s="27"/>
+      <c r="AG35" s="27"/>
+      <c r="AH35" s="27"/>
+      <c r="AI35" s="28"/>
+      <c r="AJ35" s="27">
+        <v>1</v>
+      </c>
+      <c r="AK35" s="27">
+        <v>1</v>
+      </c>
+      <c r="AL35" s="27">
+        <v>1</v>
+      </c>
+      <c r="AM35" s="27">
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="A36" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="C36">
+      <c r="B36" s="27"/>
+      <c r="C36" s="27">
         <v>1</v>
       </c>
       <c r="D36" s="8"/>
-      <c r="I36">
-        <v>1</v>
-      </c>
-      <c r="J36" s="14"/>
-      <c r="K36" s="15"/>
-      <c r="L36" s="15"/>
-      <c r="M36" s="15"/>
-      <c r="N36" s="15"/>
-      <c r="O36" s="15"/>
-      <c r="P36" s="15"/>
-      <c r="Q36" s="15"/>
-      <c r="R36" s="15"/>
-      <c r="S36" s="15"/>
-      <c r="T36" s="15"/>
-      <c r="U36" s="15"/>
-      <c r="V36" s="15"/>
-      <c r="W36" s="18"/>
-      <c r="X36" s="15"/>
-      <c r="Y36" s="8"/>
-      <c r="AI36">
-        <v>1</v>
-      </c>
-      <c r="AJ36" s="1"/>
-      <c r="AK36">
-        <v>1</v>
-      </c>
-      <c r="AL36" s="3"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
+      <c r="G36" s="27"/>
+      <c r="H36" s="27"/>
+      <c r="I36" s="3">
+        <v>1</v>
+      </c>
+      <c r="J36" s="29"/>
+      <c r="K36" s="29"/>
+      <c r="L36" s="29"/>
+      <c r="M36" s="29"/>
+      <c r="N36" s="29"/>
+      <c r="O36" s="29"/>
+      <c r="P36" s="29"/>
+      <c r="Q36" s="29"/>
+      <c r="R36" s="29"/>
+      <c r="S36" s="29"/>
+      <c r="T36" s="29"/>
+      <c r="U36" s="29"/>
+      <c r="V36" s="29"/>
+      <c r="W36" s="29"/>
+      <c r="X36" s="29"/>
+      <c r="Y36" s="27"/>
+      <c r="Z36" s="27"/>
+      <c r="AA36" s="27"/>
+      <c r="AB36" s="27"/>
+      <c r="AC36" s="27"/>
+      <c r="AD36" s="27"/>
+      <c r="AE36" s="27"/>
+      <c r="AF36" s="27"/>
+      <c r="AG36" s="27"/>
+      <c r="AH36" s="27"/>
+      <c r="AI36" s="27">
+        <v>1</v>
+      </c>
+      <c r="AJ36" s="28"/>
+      <c r="AK36" s="27">
+        <v>1</v>
+      </c>
+      <c r="AL36" s="27"/>
+      <c r="AM36" s="27"/>
     </row>
     <row r="37" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="A37" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="C37">
+      <c r="B37" s="27"/>
+      <c r="C37" s="27">
         <v>1</v>
       </c>
       <c r="D37" s="8"/>
-      <c r="J37" s="14"/>
-      <c r="K37" s="15"/>
-      <c r="L37" s="15"/>
-      <c r="M37" s="15"/>
-      <c r="N37" s="15"/>
-      <c r="O37" s="15"/>
-      <c r="P37" s="15"/>
-      <c r="Q37" s="15"/>
-      <c r="R37" s="15"/>
-      <c r="S37" s="15"/>
-      <c r="T37" s="15"/>
-      <c r="U37" s="15"/>
-      <c r="V37" s="15"/>
-      <c r="W37" s="18"/>
-      <c r="X37" s="15"/>
-      <c r="Y37" s="8"/>
-      <c r="AI37">
-        <v>1</v>
-      </c>
-      <c r="AJ37">
-        <v>1</v>
-      </c>
-      <c r="AK37" s="1"/>
-      <c r="AL37" s="2">
-        <v>1</v>
-      </c>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="27"/>
+      <c r="H37" s="27"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="29"/>
+      <c r="K37" s="29"/>
+      <c r="L37" s="29"/>
+      <c r="M37" s="29"/>
+      <c r="N37" s="29"/>
+      <c r="O37" s="29"/>
+      <c r="P37" s="29"/>
+      <c r="Q37" s="29"/>
+      <c r="R37" s="29"/>
+      <c r="S37" s="29"/>
+      <c r="T37" s="29"/>
+      <c r="U37" s="29"/>
+      <c r="V37" s="29"/>
+      <c r="W37" s="29"/>
+      <c r="X37" s="29"/>
+      <c r="Y37" s="27"/>
+      <c r="Z37" s="27"/>
+      <c r="AA37" s="27"/>
+      <c r="AB37" s="27"/>
+      <c r="AC37" s="27"/>
+      <c r="AD37" s="27"/>
+      <c r="AE37" s="27"/>
+      <c r="AF37" s="27"/>
+      <c r="AG37" s="27"/>
+      <c r="AH37" s="27"/>
+      <c r="AI37" s="27">
+        <v>1</v>
+      </c>
+      <c r="AJ37" s="27">
+        <v>1</v>
+      </c>
+      <c r="AK37" s="28"/>
+      <c r="AL37" s="27">
+        <v>1</v>
+      </c>
+      <c r="AM37" s="27"/>
     </row>
     <row r="38" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="A38" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="C38">
-        <v>1</v>
-      </c>
-      <c r="D38" s="9"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
-      <c r="J38" s="20"/>
-      <c r="K38" s="21"/>
-      <c r="L38" s="21"/>
-      <c r="M38" s="21"/>
-      <c r="N38" s="21"/>
-      <c r="O38" s="21"/>
-      <c r="P38" s="21"/>
-      <c r="Q38" s="21"/>
-      <c r="R38" s="21"/>
-      <c r="S38" s="21"/>
-      <c r="T38" s="21"/>
-      <c r="U38" s="21"/>
-      <c r="V38" s="21"/>
-      <c r="W38" s="22"/>
-      <c r="X38" s="21"/>
-      <c r="Y38" s="9"/>
-      <c r="Z38" s="2"/>
-      <c r="AA38" s="2"/>
-      <c r="AB38" s="2"/>
-      <c r="AC38" s="2"/>
-      <c r="AD38" s="2"/>
-      <c r="AE38" s="2"/>
-      <c r="AF38" s="2"/>
-      <c r="AG38" s="2"/>
-      <c r="AH38" s="2"/>
-      <c r="AI38" s="2">
-        <v>1</v>
-      </c>
-      <c r="AJ38" s="2"/>
-      <c r="AK38" s="2">
-        <v>1</v>
-      </c>
-      <c r="AL38" s="10"/>
-      <c r="AM38">
+      <c r="B38" s="27"/>
+      <c r="C38" s="27">
+        <v>1</v>
+      </c>
+      <c r="D38" s="8"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="27"/>
+      <c r="G38" s="27"/>
+      <c r="H38" s="27"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="29"/>
+      <c r="K38" s="29"/>
+      <c r="L38" s="29"/>
+      <c r="M38" s="29"/>
+      <c r="N38" s="29"/>
+      <c r="O38" s="29"/>
+      <c r="P38" s="29"/>
+      <c r="Q38" s="29"/>
+      <c r="R38" s="29"/>
+      <c r="S38" s="29"/>
+      <c r="T38" s="29"/>
+      <c r="U38" s="29"/>
+      <c r="V38" s="29"/>
+      <c r="W38" s="29"/>
+      <c r="X38" s="29"/>
+      <c r="Y38" s="27"/>
+      <c r="Z38" s="27"/>
+      <c r="AA38" s="27"/>
+      <c r="AB38" s="27"/>
+      <c r="AC38" s="27"/>
+      <c r="AD38" s="27"/>
+      <c r="AE38" s="27"/>
+      <c r="AF38" s="27"/>
+      <c r="AG38" s="27"/>
+      <c r="AH38" s="27"/>
+      <c r="AI38" s="27">
+        <v>1</v>
+      </c>
+      <c r="AJ38" s="27"/>
+      <c r="AK38" s="27">
+        <v>1</v>
+      </c>
+      <c r="AL38" s="28"/>
+      <c r="AM38" s="27">
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="A39" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="C39">
-        <v>1</v>
-      </c>
-      <c r="AE39">
-        <v>1</v>
-      </c>
-      <c r="AI39">
-        <v>1</v>
-      </c>
-      <c r="AL39">
-        <v>1</v>
-      </c>
+      <c r="B39" s="27"/>
+      <c r="C39" s="27">
+        <v>1</v>
+      </c>
+      <c r="D39" s="9"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="30"/>
+      <c r="K39" s="30"/>
+      <c r="L39" s="30"/>
+      <c r="M39" s="30"/>
+      <c r="N39" s="30"/>
+      <c r="O39" s="30"/>
+      <c r="P39" s="30"/>
+      <c r="Q39" s="30"/>
+      <c r="R39" s="30"/>
+      <c r="S39" s="30"/>
+      <c r="T39" s="30"/>
+      <c r="U39" s="30"/>
+      <c r="V39" s="30"/>
+      <c r="W39" s="30"/>
+      <c r="X39" s="30"/>
+      <c r="Y39" s="27"/>
+      <c r="Z39" s="27"/>
+      <c r="AA39" s="27"/>
+      <c r="AB39" s="27"/>
+      <c r="AC39" s="27"/>
+      <c r="AD39" s="27"/>
+      <c r="AE39" s="27">
+        <v>1</v>
+      </c>
+      <c r="AF39" s="27"/>
+      <c r="AG39" s="27"/>
+      <c r="AH39" s="27"/>
+      <c r="AI39" s="27">
+        <v>1</v>
+      </c>
+      <c r="AJ39" s="27"/>
+      <c r="AK39" s="27"/>
+      <c r="AL39" s="27">
+        <v>1</v>
+      </c>
+      <c r="AM39" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3673,9 +4250,9 @@
   <dimension ref="A1:AG33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="R1" activePane="topRight" state="frozen"/>
       <selection activeCell="B11" sqref="B11"/>
-      <selection pane="topRight" activeCell="P17" sqref="P17"/>
+      <selection pane="topRight" sqref="A1:AG33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5048,7 +5625,7 @@
   <dimension ref="A1:AN40"/>
   <sheetViews>
     <sheetView zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="AB1" sqref="AB1"/>
     </sheetView>
   </sheetViews>
@@ -8786,7 +9363,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:AO41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="C16" sqref="C16"/>
     </sheetView>

</xml_diff>